<commit_message>
uncertainty propagation code, figured out the variables
</commit_message>
<xml_diff>
--- a/data/FSR_S3/curve/FSR_S3 Curve Data.xlsx
+++ b/data/FSR_S3/curve/FSR_S3 Curve Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amro365-my.sharepoint.com/personal/pr19556_appliedmed_com/Documents/Desktop/FSR/data/FSR_S3/curve/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickruiz/Desktop/FSR/data/FSR_S3/curve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="13_ncr:1_{28B33FDE-C65A-4F48-9078-D0680499B51D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6590150B-5262-4A57-9AE2-DAFE51C00621}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9376CF8A-3625-8243-AB51-335AA7A5B536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6660" yWindow="1095" windowWidth="21600" windowHeight="11160" xr2:uid="{A44B9C34-151F-4DB5-ABDC-540135FA09DD}"/>
+    <workbookView xWindow="6660" yWindow="1100" windowWidth="21600" windowHeight="11160" xr2:uid="{A44B9C34-151F-4DB5-ABDC-540135FA09DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -106,7 +106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -117,14 +117,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -147,9 +141,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -187,7 +181,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -293,7 +287,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -435,7 +429,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -446,24 +440,24 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="3"/>
-    <col min="2" max="2" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="3"/>
-    <col min="5" max="5" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="8.83203125" style="3"/>
+    <col min="2" max="2" width="14.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="3"/>
+    <col min="5" max="5" width="8.83203125" style="1"/>
     <col min="6" max="6" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="3"/>
+    <col min="7" max="7" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -488,132 +482,132 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="1">
         <v>18610.34245</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="1">
         <v>117.69955</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="1">
         <v>-0.94469999999999998</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="1">
         <v>3.4399999999999999E-3</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="1">
         <v>11947.817849999999</v>
       </c>
-      <c r="H2" s="4"/>
+      <c r="H2" s="1"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>19780.028689999999</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>112.43103000000001</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>-0.97023000000000004</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>3.0799999999999998E-3</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>1</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>9825.19247</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>18849.235840000001</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>106.90512</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>-0.94596999999999998</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>3.0799999999999998E-3</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>1</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>9878.9868299999998</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="1">
         <v>17337.01756</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="1">
         <v>106.54469</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="1">
         <v>-0.90935999999999995</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="1">
         <v>3.3300000000000001E-3</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="1">
         <v>10916.393389999999</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="1">
         <v>17347.315070000001</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="1">
         <v>92.1691</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="1">
         <v>-0.90005000000000002</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="1">
         <v>2.8800000000000002E-3</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="1">
         <v>1</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="1">
         <v>8368.0072099999998</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -637,7 +631,7 @@
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -661,7 +655,7 @@
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -685,7 +679,7 @@
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -708,11 +702,11 @@
         <v>8252.0395800000006</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="5">
         <v>15555.82482</v>
       </c>
       <c r="C11" s="1">

</xml_diff>